<commit_message>
Edit format tipe rumah
</commit_message>
<xml_diff>
--- a/public/downloads/Format_Import_Data_Tipe_Rumah.xlsx
+++ b/public/downloads/Format_Import_Data_Tipe_Rumah.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="63">
   <si>
     <t>no</t>
   </si>
@@ -23,94 +23,184 @@
     <t>harga_sewa</t>
   </si>
   <si>
+    <t>terbilang</t>
+  </si>
+  <si>
     <t>II/250</t>
   </si>
   <si>
+    <t>Satu Juta Lima Ratus Tiga Puluh Satu Ribu Sembilan Ratus Enam Puluh Lima Rupiah</t>
+  </si>
+  <si>
     <t>II/220</t>
   </si>
   <si>
+    <t>Satu Juta Tiga Ratus Empat Puluh Delapan Ribu Dua Ratus Rupiah</t>
+  </si>
+  <si>
     <t>II/190</t>
   </si>
   <si>
+    <t>Satu Juta Seratus Enam Puluh Empat Ribu Tiga Ratus Rupiah</t>
+  </si>
+  <si>
     <t>II/180</t>
   </si>
   <si>
+    <t>Satu Juta Seratus Tiga Ribu Seratus Rupiah</t>
+  </si>
+  <si>
     <t>II/175</t>
   </si>
   <si>
+    <t>Satu Juta Dua Puluh Tujuh Ribu Lima Ratus Rupiah</t>
+  </si>
+  <si>
     <t>II/165</t>
   </si>
   <si>
+    <t>Satu Juta Sebelas Ribu Tiga Ratus Rupiah</t>
+  </si>
+  <si>
     <t>II/150</t>
   </si>
   <si>
+    <t>Sembilan Ratus Sembilan Belas Ribu Dua Ratus Rupiah</t>
+  </si>
+  <si>
     <t>II/148</t>
   </si>
   <si>
+    <t>Sembilan Ratus Enam Ribu Sembilan Ratus Rupiah</t>
+  </si>
+  <si>
     <t>II/142</t>
   </si>
   <si>
+    <t>Delapan Ratus Tujuh Puluh Ribu Seratus Lima Puluh Rupiah</t>
+  </si>
+  <si>
     <t>II/140</t>
   </si>
   <si>
+    <t>Delapan Ratus Lima Puluh Delapan Ribu Rupiah</t>
+  </si>
+  <si>
     <t>II/135</t>
   </si>
   <si>
     <t>II/123</t>
   </si>
   <si>
+    <t>Tujuh Ratus Lima Puluh TIga Ribu Tujuh Ratus Lima Puluh Rupiah</t>
+  </si>
+  <si>
     <t>II/120</t>
   </si>
   <si>
+    <t>Tujuh Ratus Tiga Puluh Lima Ribu Tiga Ratus Empat Puluh Lima Rupiah</t>
+  </si>
+  <si>
     <t>II/115</t>
   </si>
   <si>
+    <t>Tujuh Ratus Empat Ribu Tujuh Ratus Rupiah</t>
+  </si>
+  <si>
     <t>II/100</t>
   </si>
   <si>
+    <t>Enam Ratus Dua Belas Ribu Rupiah</t>
+  </si>
+  <si>
     <t>II/96</t>
   </si>
   <si>
+    <t>Lima Rates Delapan Puluh Delapan Ribu Rupiah</t>
+  </si>
+  <si>
     <t>II/90</t>
   </si>
   <si>
+    <t>Empat Ratus Lima Puluh Sembilan Ribu Enam Ratus Rupiah</t>
+  </si>
+  <si>
     <t>II/86</t>
   </si>
   <si>
+    <t>Empat Ratus Tiga Puluh Sembilan Ribu Dua Ratus Rupiah</t>
+  </si>
+  <si>
     <t>II/80</t>
   </si>
   <si>
+    <t>Empar Ratus Delapan Ribu Empat Ratus Lima Puluh Rupiah</t>
+  </si>
+  <si>
     <t>II/75</t>
   </si>
   <si>
+    <t>Tiga Ratus Delapan Puluh Dua Sembilan Ratus Lima Puluh</t>
+  </si>
+  <si>
     <t>II/70</t>
   </si>
   <si>
+    <t>Tiga Ratus Lima Puluh Tujuh Ribu Empat Ratus Lima Rupiah</t>
+  </si>
+  <si>
     <t>II/66</t>
   </si>
   <si>
+    <t>Tiga Ratus Tiga Puluh Enam Ribu Sembilan Ratus Rupiah</t>
+  </si>
+  <si>
     <t>II/65</t>
   </si>
   <si>
+    <t>Tiga Ratus Tiga Puluh Satu Ribu Delapan Ratus Tujuh Puluh Lima Rupiah</t>
+  </si>
+  <si>
     <t>II/60</t>
   </si>
   <si>
+    <t>Tiga Ratus Enam Ribu Empat Ratus Lima Puluh Rupiah</t>
+  </si>
+  <si>
     <t>II/54</t>
   </si>
   <si>
+    <t>Dua Ratus Tujuh Puluh Lima Ribu Tujuh Ratus Rupiah</t>
+  </si>
+  <si>
     <t>II/50</t>
   </si>
   <si>
+    <t>Dua Ratus Lima Puluh Lima Ribu Tiga Ratus Rupiah</t>
+  </si>
+  <si>
     <t>II/45</t>
   </si>
   <si>
+    <t>Dua Ratus Dua Puluh Sembilan Ribu Delapan Ratus Rupiah</t>
+  </si>
+  <si>
     <t>II/40</t>
   </si>
   <si>
+    <t>Dua Ratus Empat Ribu Rupiah</t>
+  </si>
+  <si>
     <t>II/36</t>
   </si>
   <si>
+    <t>Seratus Delapan Puluh Tiga Ribu Sempbilan Ratus Rupiah</t>
+  </si>
+  <si>
     <t>II/21</t>
+  </si>
+  <si>
+    <t>Tiga Puluh Enam Ribu Rupiah</t>
   </si>
 </sst>
 </file>
@@ -120,7 +210,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -128,6 +218,11 @@
     </font>
     <font>
       <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="13"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
     </font>
@@ -192,23 +287,26 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="4" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -246,10 +344,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="404040"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="BFBFBF"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="499BC9"/>
@@ -443,14 +541,15 @@
   <a:objectDefaults>
     <a:spDef>
       <a:spPr>
-        <a:blipFill rotWithShape="1">
-          <a:blip r:embed="rId1"/>
-          <a:srcRect l="0" t="0" r="0" b="0"/>
-          <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
-        </a:blipFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst>
           <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
@@ -465,35 +564,29 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst>
-              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
-                <a:srgbClr val="000000">
-                  <a:alpha val="31034"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
             <a:uFillTx/>
             <a:latin typeface="+mn-lt"/>
             <a:ea typeface="+mn-ea"/>
@@ -746,14 +839,20 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="6350" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
-        <a:effectLst/>
+        <a:effectLst>
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:srgbClr val="000000">
+              <a:alpha val="50000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -1042,7 +1141,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1323,18 +1422,17 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.6" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="19.6016" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.6016" style="1" customWidth="1"/>
     <col min="3" max="3" width="19.6016" style="1" customWidth="1"/>
-    <col min="4" max="256" width="19.6016" style="1" customWidth="1"/>
+    <col min="4" max="4" width="87.9844" style="1" customWidth="1"/>
+    <col min="5" max="256" width="19.6016" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="21" customHeight="1">
@@ -1347,16 +1445,22 @@
       <c r="C1" t="s" s="2">
         <v>2</v>
       </c>
+      <c r="D1" t="s" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" ht="14.5" customHeight="1">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" t="s" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="5">
         <v>1531965</v>
+      </c>
+      <c r="D2" t="s" s="6">
+        <v>5</v>
       </c>
     </row>
     <row r="3" ht="14.5" customHeight="1">
@@ -1364,10 +1468,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" s="5">
         <v>1348200</v>
+      </c>
+      <c r="D3" t="s" s="6">
+        <v>7</v>
       </c>
     </row>
     <row r="4" ht="14.5" customHeight="1">
@@ -1375,10 +1482,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s" s="4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C4" s="5">
         <v>1164300</v>
+      </c>
+      <c r="D4" t="s" s="6">
+        <v>9</v>
       </c>
     </row>
     <row r="5" ht="14.5" customHeight="1">
@@ -1386,10 +1496,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s" s="4">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C5" s="5">
         <v>1103100</v>
+      </c>
+      <c r="D5" t="s" s="6">
+        <v>11</v>
       </c>
     </row>
     <row r="6" ht="14.5" customHeight="1">
@@ -1397,10 +1510,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s" s="4">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C6" s="5">
         <v>1027500</v>
+      </c>
+      <c r="D6" t="s" s="6">
+        <v>13</v>
       </c>
     </row>
     <row r="7" ht="14.5" customHeight="1">
@@ -1408,10 +1524,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s" s="4">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C7" s="5">
         <v>1011300</v>
+      </c>
+      <c r="D7" t="s" s="6">
+        <v>15</v>
       </c>
     </row>
     <row r="8" ht="14.5" customHeight="1">
@@ -1419,10 +1538,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s" s="4">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C8" s="5">
         <v>919200</v>
+      </c>
+      <c r="D8" t="s" s="6">
+        <v>17</v>
       </c>
     </row>
     <row r="9" ht="14.5" customHeight="1">
@@ -1430,10 +1552,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s" s="4">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C9" s="5">
         <v>906900</v>
+      </c>
+      <c r="D9" t="s" s="6">
+        <v>19</v>
       </c>
     </row>
     <row r="10" ht="14.5" customHeight="1">
@@ -1441,10 +1566,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s" s="4">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C10" s="5">
         <v>870150</v>
+      </c>
+      <c r="D10" t="s" s="6">
+        <v>21</v>
       </c>
     </row>
     <row r="11" ht="14.5" customHeight="1">
@@ -1452,10 +1580,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s" s="4">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C11" s="5">
         <v>858000</v>
+      </c>
+      <c r="D11" t="s" s="6">
+        <v>23</v>
       </c>
     </row>
     <row r="12" ht="14.5" customHeight="1">
@@ -1463,10 +1594,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s" s="4">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C12" s="5">
         <v>827250</v>
+      </c>
+      <c r="D12" t="s" s="6">
+        <v>23</v>
       </c>
     </row>
     <row r="13" ht="14.5" customHeight="1">
@@ -1474,10 +1608,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s" s="4">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C13" s="5">
         <v>753750</v>
+      </c>
+      <c r="D13" t="s" s="6">
+        <v>26</v>
       </c>
     </row>
     <row r="14" ht="14.5" customHeight="1">
@@ -1485,10 +1622,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s" s="4">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C14" s="5">
         <v>735345</v>
+      </c>
+      <c r="D14" t="s" s="6">
+        <v>28</v>
       </c>
     </row>
     <row r="15" ht="14.5" customHeight="1">
@@ -1496,10 +1636,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s" s="4">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C15" s="5">
         <v>704700</v>
+      </c>
+      <c r="D15" t="s" s="6">
+        <v>30</v>
       </c>
     </row>
     <row r="16" ht="14.5" customHeight="1">
@@ -1507,10 +1650,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s" s="4">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C16" s="5">
         <v>612000</v>
+      </c>
+      <c r="D16" t="s" s="6">
+        <v>32</v>
       </c>
     </row>
     <row r="17" ht="14.5" customHeight="1">
@@ -1518,10 +1664,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s" s="4">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="C17" s="5">
         <v>588000</v>
+      </c>
+      <c r="D17" t="s" s="6">
+        <v>34</v>
       </c>
     </row>
     <row r="18" ht="14.5" customHeight="1">
@@ -1529,10 +1678,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s" s="4">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="C18" s="5">
         <v>459600</v>
+      </c>
+      <c r="D18" t="s" s="6">
+        <v>36</v>
       </c>
     </row>
     <row r="19" ht="14.5" customHeight="1">
@@ -1540,10 +1692,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s" s="4">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="C19" s="5">
         <v>439200</v>
+      </c>
+      <c r="D19" t="s" s="6">
+        <v>38</v>
       </c>
     </row>
     <row r="20" ht="14.5" customHeight="1">
@@ -1551,10 +1706,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s" s="4">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="C20" s="5">
         <v>408450</v>
+      </c>
+      <c r="D20" t="s" s="6">
+        <v>40</v>
       </c>
     </row>
     <row r="21" ht="14.5" customHeight="1">
@@ -1562,10 +1720,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s" s="4">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="C21" s="5">
         <v>382950</v>
+      </c>
+      <c r="D21" t="s" s="6">
+        <v>42</v>
       </c>
     </row>
     <row r="22" ht="14.5" customHeight="1">
@@ -1573,10 +1734,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s" s="4">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="C22" s="5">
         <v>357405</v>
+      </c>
+      <c r="D22" t="s" s="6">
+        <v>44</v>
       </c>
     </row>
     <row r="23" ht="14.5" customHeight="1">
@@ -1584,10 +1748,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s" s="4">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="C23" s="5">
         <v>336900</v>
+      </c>
+      <c r="D23" t="s" s="6">
+        <v>46</v>
       </c>
     </row>
     <row r="24" ht="14.5" customHeight="1">
@@ -1595,10 +1762,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s" s="4">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="C24" s="5">
         <v>331875</v>
+      </c>
+      <c r="D24" t="s" s="6">
+        <v>48</v>
       </c>
     </row>
     <row r="25" ht="14.5" customHeight="1">
@@ -1606,10 +1776,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s" s="4">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="C25" s="5">
         <v>306450</v>
+      </c>
+      <c r="D25" t="s" s="6">
+        <v>50</v>
       </c>
     </row>
     <row r="26" ht="14.5" customHeight="1">
@@ -1617,10 +1790,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s" s="4">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C26" s="5">
         <v>275700</v>
+      </c>
+      <c r="D26" t="s" s="6">
+        <v>52</v>
       </c>
     </row>
     <row r="27" ht="14.5" customHeight="1">
@@ -1628,10 +1804,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s" s="4">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="C27" s="5">
         <v>255300</v>
+      </c>
+      <c r="D27" t="s" s="6">
+        <v>54</v>
       </c>
     </row>
     <row r="28" ht="14.5" customHeight="1">
@@ -1639,10 +1818,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s" s="4">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="C28" s="5">
         <v>229800</v>
+      </c>
+      <c r="D28" t="s" s="6">
+        <v>56</v>
       </c>
     </row>
     <row r="29" ht="14.5" customHeight="1">
@@ -1650,10 +1832,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s" s="4">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="C29" s="5">
         <v>204000</v>
+      </c>
+      <c r="D29" t="s" s="6">
+        <v>58</v>
       </c>
     </row>
     <row r="30" ht="14.5" customHeight="1">
@@ -1661,10 +1846,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s" s="4">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="C30" s="5">
         <v>183900</v>
+      </c>
+      <c r="D30" t="s" s="6">
+        <v>60</v>
       </c>
     </row>
     <row r="31" ht="14.5" customHeight="1">
@@ -1672,10 +1860,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s" s="4">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="C31" s="5">
         <v>36000</v>
+      </c>
+      <c r="D31" t="s" s="6">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>